<commit_message>
Update faqs.xlsx and add data logging file
</commit_message>
<xml_diff>
--- a/faqs.xlsx
+++ b/faqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chosr\OneDrive - Seethabharatgas\SRI\Documents\whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75E7AB2-37CB-463B-8DEA-8624E312EC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5774EA-D40C-466C-A9EE-D98CB4BDFFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Question</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>Who is animal husbandry Secretary</t>
   </si>
 </sst>
 </file>
@@ -354,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,6 +385,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update FAQ database with new questions and answers
</commit_message>
<xml_diff>
--- a/faqs.xlsx
+++ b/faqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chosr\OneDrive - Seethabharatgas\SRI\Documents\whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8AE77-1266-438D-8586-2D278DC52F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D471572A-7632-4482-BFDF-004E3858AF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="172">
   <si>
     <t>Question</t>
   </si>
@@ -564,6 +564,231 @@
       </rPr>
       <t>Homogenization is a process that breaks down fat globules, preventing cream from separating and rising to the top.</t>
     </r>
+  </si>
+  <si>
+    <t>Which animals should not be vaccinated?</t>
+  </si>
+  <si>
+    <t>Sick animals, newborn calves, and young animals up to 3–4 months old should not be vaccinated.</t>
+  </si>
+  <si>
+    <t>Can pregnant animals be vaccinated?</t>
+  </si>
+  <si>
+    <t>Yes, pregnant animals can be vaccinated, except during the advanced stage of pregnancy, when it should be avoided.</t>
+  </si>
+  <si>
+    <t>Can all types of vaccines be given to pregnant animals?</t>
+  </si>
+  <si>
+    <t>Generally, yes. If any vaccine is unsuitable, veterinarians will not administer it. Always consult a veterinarian before vaccination.</t>
+  </si>
+  <si>
+    <t>Can multiple vaccines be given at the same time?</t>
+  </si>
+  <si>
+    <t>Yes, animals can be vaccinated against more than one disease at the same time.</t>
+  </si>
+  <si>
+    <t>Do symptoms like swelling, lumps on the neck, reduced milk, bloating, or lameness occur after vaccination?</t>
+  </si>
+  <si>
+    <t>Yes, often in weak animals. Vaccination can cause temporary stress leading to reduced milk, less appetite, or bloating. Swelling or lumps should be treated with ice packs. These symptoms usually reduce after basic treatment.</t>
+  </si>
+  <si>
+    <t>What is the right time for vaccination?</t>
+  </si>
+  <si>
+    <t>When does immunity develop after vaccination?</t>
+  </si>
+  <si>
+    <t>Immunity develops within 7 to 14 days after vaccination.</t>
+  </si>
+  <si>
+    <t>Is brucellosis vaccination necessary? Who should get it, and what are the benefits?</t>
+  </si>
+  <si>
+    <t>Yes, female animals aged 4–8 months should be vaccinated once. This prevents abortions during mid to late pregnancy.</t>
+  </si>
+  <si>
+    <t>Which animal bites require rabies vaccination?</t>
+  </si>
+  <si>
+    <t>Bites from dogs, cats, rabid animals, monkeys, wolves, mongooses, or any wild animals require rabies vaccination.</t>
+  </si>
+  <si>
+    <t>What should be done if bitten by a rabid dog or wild animal?</t>
+  </si>
+  <si>
+    <t>Wash the wound under running water for 10–15 minutes, clean with soap, apply iodine, and immediately visit the nearest hospital.</t>
+  </si>
+  <si>
+    <t>Does taking only one or two doses of rabies vaccine help after a dog bite?</t>
+  </si>
+  <si>
+    <t>No, the full rabies vaccine course is absolutely necessary.</t>
+  </si>
+  <si>
+    <t>Should deworming be done before vaccination?</t>
+  </si>
+  <si>
+    <t>Yes, deworming one week before vaccination increases its effectiveness.</t>
+  </si>
+  <si>
+    <t>Can rabies still occur if the biting animal was vaccinated?</t>
+  </si>
+  <si>
+    <t>Yes, but the chances are very low.</t>
+  </si>
+  <si>
+    <t>Can rabies spread from drinking milk of an infected animal?</t>
+  </si>
+  <si>
+    <t>Yes, it can. If the milk is boiled thoroughly, the risk is reduced. However, milk from rabid animals should not be consumed.</t>
+  </si>
+  <si>
+    <t>Should people handling rabid animals be vaccinated?</t>
+  </si>
+  <si>
+    <t>Yes, anyone handling rabid animals must get rabies vaccination.</t>
+  </si>
+  <si>
+    <t>What should be done if a snake bites an animal?</t>
+  </si>
+  <si>
+    <t>Tie a tight band 3–4 inches above the bite to stop blood circulation, make a small cut with a sterile blade to let out contaminated blood, wash with clean water, and immediately call 1962 helpline or contact the nearest veterinarian.</t>
+  </si>
+  <si>
+    <t>What should be done if an animal suffers from bloating?</t>
+  </si>
+  <si>
+    <t>Stop feeding, give 500 ml edible oil + 30 ml turpentine oil + black salt slowly, and contact the nearest vet via helpline 1962.</t>
+  </si>
+  <si>
+    <t>What if bloating occurs after eating tender green fodder?</t>
+  </si>
+  <si>
+    <t>Stop green fodder, provide dry fodder, give 500 ml edible oil + 35 ml turpentine oil + black salt slowly, and contact the vet immediately through helpline 1962.</t>
+  </si>
+  <si>
+    <t>Can stale food or flour be fed to animals?</t>
+  </si>
+  <si>
+    <t>No, stale food and flour can cause indigestion, bloating, and poisoning.</t>
+  </si>
+  <si>
+    <t>What should be done if an animal is poisoned from food?</t>
+  </si>
+  <si>
+    <t>Stop feeding, give baking soda or vinegar mixed with water immediately.</t>
+  </si>
+  <si>
+    <t>Should vaccination be done if vaccines were not stored in cold chain?</t>
+  </si>
+  <si>
+    <t>No, vaccines must always be kept in cold storage (cold chain).</t>
+  </si>
+  <si>
+    <t>How to maintain good animal health and productivity?</t>
+  </si>
+  <si>
+    <t>Regular deworming, vaccination, clean housing, clean drinking water, and proper hygiene to prevent ticks and disease spread.</t>
+  </si>
+  <si>
+    <t>What to do if animals are poisoned?</t>
+  </si>
+  <si>
+    <t>1. If due to tick medicine (cypermethrin), wash the animal thoroughly and give 50–100 g charcoal powder. 2. If due to sorghum stems or onion leaves, give lime water, charcoal powder, or vinegar. 3. Immediately call helpline 1962 or a nearby vet.</t>
+  </si>
+  <si>
+    <t>How much colostrum should a newborn calf receive and when?</t>
+  </si>
+  <si>
+    <t>Within the first few hours of birth, feed colostrum equal to 10% of the calf’s body weight.</t>
+  </si>
+  <si>
+    <t>What should be done if an animal develops mastitis?</t>
+  </si>
+  <si>
+    <t>Home remedy: Mix 250 g aloe vera, 50 g turmeric, 15 g lime, and 150–200 ml water into a paste. Apply on the udder 10 times a day for 5 days. Also, immediately contact helpline 1962 or a vet.</t>
+  </si>
+  <si>
+    <t>How much feed should be given to pregnant animals?</t>
+  </si>
+  <si>
+    <t>Along with regular fodder, provide an extra 3–4 kg fodder and 1–2 kg oil cakes.</t>
+  </si>
+  <si>
+    <t>What extra feed should be given to lactating animals?</t>
+  </si>
+  <si>
+    <t>Give 1–2 kg concentrate (oil cake).</t>
+  </si>
+  <si>
+    <t>How to make low-quality fodder nutritious?</t>
+  </si>
+  <si>
+    <t>Treat it with urea. Cut into 1–2 inch pieces, spread on plastic, spray with a solution of 4 kg urea in 40 liters water per 100 kg fodder, keep airtight for 2–3 weeks, then feed. This increases digestibility and nutrition.</t>
+  </si>
+  <si>
+    <t>When can calves be given feed apart from milk?</t>
+  </si>
+  <si>
+    <t>From 6–8 weeks onwards, small amounts of fodder can be introduced.</t>
+  </si>
+  <si>
+    <t>When should deworming medicine be given to calves?</t>
+  </si>
+  <si>
+    <t>On the 6th–10th day after birth, then monthly up to 6 months, and afterwards every 3–4 months (summer, rainy season, winter) — three times a year.</t>
+  </si>
+  <si>
+    <t>When should castration be done?</t>
+  </si>
+  <si>
+    <t>Within the first year of life.</t>
+  </si>
+  <si>
+    <t>What is Artificial Insemination (AI)?</t>
+  </si>
+  <si>
+    <t>It is fertilization carried out scientifically without natural mating.</t>
+  </si>
+  <si>
+    <t>At what age do female animals become pregnant?</t>
+  </si>
+  <si>
+    <t>Crossbred cows: 8 months–1 year; Local cows: 2.5–3 years.</t>
+  </si>
+  <si>
+    <t>How to identify heat signs in female animals?</t>
+  </si>
+  <si>
+    <t>Frequent urination, swollen and reddish vulva, transparent discharge, restlessness, reduced appetite, and mounting other animals.</t>
+  </si>
+  <si>
+    <t>When should AI be performed?</t>
+  </si>
+  <si>
+    <t>In the mid-heat stage (10–12 hours after onset).</t>
+  </si>
+  <si>
+    <t>What is the success rate of AI?</t>
+  </si>
+  <si>
+    <t>40–60% or higher with good quality semen from approved bulls, properly timed.</t>
+  </si>
+  <si>
+    <t>Should animals be allowed to mate naturally after AI?</t>
+  </si>
+  <si>
+    <t>No, if AI is done properly, natural mating should not be allowed.</t>
+  </si>
+  <si>
+    <t>Which semen varieties are available for AI in Maharashtra?</t>
+  </si>
+  <si>
+    <t>Cows: Holstein Friesian (HF-100%), Jersey (JR-100%), crossbred HF &amp; JR, Deoni, Lal Kandhari, Gir, Sahiwal, Khillari. Buffaloes: Murrah, Surti, Jaffrabadi.</t>
   </si>
 </sst>
 </file>
@@ -630,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -647,6 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,39 +1153,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="217.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="217.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1517,6 +1744,307 @@
       </c>
       <c r="B96" s="1" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>